<commit_message>
[UPDATE] now it has a short sign
</commit_message>
<xml_diff>
--- a/backend/data/data.xlsx
+++ b/backend/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node.js Apps\funding-rate-flip-prototype\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node.js Apps\funding-rate-flip-prototype\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C847AD77-2CED-4AC7-B89B-3E87C58C1829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930608E0-A1D6-4784-9952-A61C280B979B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,7 +409,7 @@
         <v>30000</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="E3">
         <v>18090</v>
@@ -423,13 +423,13 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>600000</v>
+        <v>-1000</v>
       </c>
       <c r="D4">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>18090</v>
+        <v>16280</v>
       </c>
       <c r="F4">
         <v>1000000</v>

</xml_diff>

<commit_message>
[FIX] bug on short and long checking
</commit_message>
<xml_diff>
--- a/backend/data/data.xlsx
+++ b/backend/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Node.js Apps\funding-rate-flip-prototype\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930608E0-A1D6-4784-9952-A61C280B979B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C370A1-ABAB-4BF6-9B62-5796F53984E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,13 +409,13 @@
         <v>30000</v>
       </c>
       <c r="D3">
-        <v>-0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E3">
         <v>18090</v>
       </c>
       <c r="F3">
-        <v>1000000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -423,16 +423,16 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>-1000</v>
+        <v>30000</v>
       </c>
       <c r="D4">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="E4">
-        <v>16280</v>
+        <v>18090</v>
       </c>
       <c r="F4">
-        <v>1000000</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>